<commit_message>
Reimplemented PHP's CSV read functionality so we do not have locale bugs
</commit_message>
<xml_diff>
--- a/_tests/assets/spreadsheets/test.xlsx
+++ b/_tests/assets/spreadsheets/test.xlsx
@@ -37,7 +37,7 @@
     <t xml:space="preserve">B1</t>
   </si>
   <si>
-    <t xml:space="preserve">C1</t>
+    <t xml:space="preserve">C,"1</t>
   </si>
   <si>
     <t xml:space="preserve">A2</t>
@@ -46,10 +46,11 @@
     <t xml:space="preserve">B2</t>
   </si>
   <si>
-    <t xml:space="preserve">C2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C3</t>
+    <t xml:space="preserve">C"2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C3
+C3</t>
   </si>
   <si>
     <t xml:space="preserve">A4</t>
@@ -67,6 +68,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -88,6 +90,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -132,13 +135,21 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -161,13 +172,10 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -181,34 +189,34 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C5" s="0" t="s">
+    <row r="5" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C5" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>